<commit_message>
Made the process iterative
</commit_message>
<xml_diff>
--- a/dse/preliminary/Tiltrotor_examples.xlsx
+++ b/dse/preliminary/Tiltrotor_examples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javia\OneDrive\Escritorio\TUDelft\Bsc 3\DSE\GitRep\dse\preliminary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523D7EDD-5FB0-42D1-881C-8DBDE57B35BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A84F3E9-3321-463B-A7A7-56C86B8263D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Pure Helicopter" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="Relarionships" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
+    <sheet name="Helicopters" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="91">
   <si>
     <t>HELICOPTER SIZING</t>
   </si>
@@ -134,12 +135,6 @@
     <t>Jane's All the world aircraft</t>
   </si>
   <si>
-    <t>Leonardo Helicopters Project Zero</t>
-  </si>
-  <si>
-    <t>https://evtol.news/agustawestland-project-zero/</t>
-  </si>
-  <si>
     <t>HIGE</t>
   </si>
   <si>
@@ -252,13 +247,79 @@
   </si>
   <si>
     <t>std = [379.9, 0.0946, 1006.32]</t>
+  </si>
+  <si>
+    <t>Shaft power = 0.41MTOM - 103.31</t>
+  </si>
+  <si>
+    <t>std = [0.042, 493.7]</t>
+  </si>
+  <si>
+    <t>R2=0.9699</t>
+  </si>
+  <si>
+    <t>std = [0.1758, 775.26]</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Max payload</t>
+  </si>
+  <si>
+    <t>CH-47</t>
+  </si>
+  <si>
+    <t>EC135-P1</t>
+  </si>
+  <si>
+    <t>EC135-635</t>
+  </si>
+  <si>
+    <t>NH90-NFH</t>
+  </si>
+  <si>
+    <t>Leonardo AW101</t>
+  </si>
+  <si>
+    <t>MTOM = 1.979*m_payload+1642.6</t>
+  </si>
+  <si>
+    <t>R2=0.9502</t>
+  </si>
+  <si>
+    <t>std = [0.2616, 1663.29]</t>
+  </si>
+  <si>
+    <t>Shaft power</t>
+  </si>
+  <si>
+    <t>Class 1 estimations</t>
+  </si>
+  <si>
+    <t>Rotor diam</t>
+  </si>
+  <si>
+    <t>Useful mass</t>
+  </si>
+  <si>
+    <t>Fuel mass</t>
+  </si>
+  <si>
+    <t>fuselage_length</t>
+  </si>
+  <si>
+    <t>Payload+ astronauts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="#,##0.0000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,21 +335,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -300,23 +371,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,6 +405,971 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.057742782152231E-3"/>
+                  <c:y val="-3.0511081948089842E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Helicopters!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>12284</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Helicopters!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>24494</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2910</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2980</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E8F9-4654-8900-2FCA230072C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="339366400"/>
+        <c:axId val="339358720"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="339366400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="339358720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="339358720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="339366400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60FE121A-72C8-855D-BE9F-A319D1DFA5A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -762,10 +1802,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B61A3E-9A50-4D31-9D62-BD187643A944}">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +1817,7 @@
     <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -787,60 +1827,63 @@
     <col min="15" max="15" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -856,7 +1899,7 @@
       <c r="G2">
         <v>5443</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>12000</v>
       </c>
       <c r="I2">
@@ -874,13 +1917,16 @@
       <c r="N2">
         <v>1830</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -899,7 +1945,7 @@
         <f>D3-4763</f>
         <v>2857</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <f>1940*2</f>
         <v>3880</v>
       </c>
@@ -930,143 +1976,181 @@
       <c r="Q3">
         <v>11.7</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>23859</v>
+      </c>
+      <c r="E4">
+        <v>3493</v>
+      </c>
+      <c r="F4">
+        <f>G4-E4</f>
+        <v>5579</v>
+      </c>
+      <c r="G4">
+        <v>9072</v>
+      </c>
+      <c r="H4" s="5">
+        <v>12000</v>
+      </c>
+      <c r="I4">
+        <v>1759</v>
       </c>
       <c r="J4">
-        <v>500</v>
+        <v>476</v>
       </c>
       <c r="K4">
-        <v>3</v>
+        <v>11.61</v>
       </c>
       <c r="M4">
-        <v>7315</v>
+        <v>7530</v>
+      </c>
+      <c r="P4">
+        <v>113.2</v>
       </c>
       <c r="Q4">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>14.02</v>
+      </c>
+      <c r="R4">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>23859</v>
-      </c>
-      <c r="E5">
-        <v>3493</v>
+        <v>1021</v>
       </c>
       <c r="F5">
-        <f>G5-E5</f>
-        <v>5579</v>
-      </c>
-      <c r="G5">
-        <v>9072</v>
-      </c>
-      <c r="H5" s="6">
-        <v>12000</v>
+        <v>227</v>
       </c>
       <c r="I5">
-        <v>1759</v>
+        <f>J5*4</f>
+        <v>2224</v>
       </c>
       <c r="J5">
-        <v>476</v>
-      </c>
-      <c r="K5">
-        <v>11.61</v>
+        <v>556</v>
       </c>
       <c r="M5">
-        <v>7530</v>
-      </c>
-      <c r="P5">
-        <v>113.2</v>
+        <v>6095</v>
       </c>
       <c r="Q5">
-        <v>14.02</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <v>5.33</v>
+      </c>
+      <c r="R5">
+        <v>4.42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
         <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>31</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1021</v>
-      </c>
-      <c r="F6">
-        <v>227</v>
+        <v>13000</v>
+      </c>
+      <c r="G6">
+        <v>5900</v>
+      </c>
+      <c r="H6" s="4">
+        <v>5500</v>
       </c>
       <c r="I6">
-        <f>J6*4</f>
-        <v>2224</v>
+        <v>2600</v>
       </c>
       <c r="J6">
-        <v>556</v>
+        <v>460</v>
+      </c>
+      <c r="K6">
+        <v>9.1</v>
       </c>
       <c r="M6">
-        <v>6095</v>
+        <v>7600</v>
       </c>
       <c r="Q6">
-        <v>5.33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="R6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>13000</v>
+        <v>1020</v>
+      </c>
+      <c r="E7">
+        <f>G7-F7</f>
+        <v>227</v>
+      </c>
+      <c r="F7">
+        <v>136</v>
       </c>
       <c r="G7">
-        <v>5900</v>
-      </c>
-      <c r="H7" s="5">
-        <v>5500</v>
+        <v>363</v>
+      </c>
+      <c r="H7" s="4">
+        <v>450</v>
       </c>
       <c r="I7">
-        <v>2600</v>
+        <f>3.54*J7</f>
+        <v>1309.8</v>
       </c>
       <c r="J7">
-        <v>460</v>
+        <v>370</v>
       </c>
       <c r="K7">
-        <v>9.1</v>
+        <v>2.9</v>
       </c>
       <c r="M7">
-        <v>7600</v>
+        <v>6100</v>
+      </c>
+      <c r="N7">
+        <v>3050</v>
       </c>
       <c r="Q7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <v>4.63</v>
+      </c>
+      <c r="R7">
+        <v>5.46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
         <v>31</v>
@@ -1075,20 +2159,20 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1020</v>
+        <v>1360</v>
       </c>
       <c r="E8">
         <f>G8-F8</f>
-        <v>227</v>
+        <v>391</v>
       </c>
       <c r="F8">
         <v>136</v>
       </c>
       <c r="G8">
-        <v>363</v>
+        <v>527</v>
       </c>
       <c r="H8" s="5">
-        <v>450</v>
+        <v>641</v>
       </c>
       <c r="I8">
         <f>3.54*J8</f>
@@ -1098,7 +2182,7 @@
         <v>370</v>
       </c>
       <c r="K8">
-        <v>2.9</v>
+        <v>3.05</v>
       </c>
       <c r="M8">
         <v>6100</v>
@@ -1107,169 +2191,307 @@
         <v>3050</v>
       </c>
       <c r="Q8">
-        <v>4.63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+        <v>4.32</v>
+      </c>
+      <c r="R8">
+        <v>5.46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>1360</v>
-      </c>
-      <c r="E9">
-        <f>G9-F9</f>
-        <v>391</v>
-      </c>
-      <c r="F9">
-        <v>136</v>
+        <v>1451</v>
       </c>
       <c r="G9">
-        <v>527</v>
-      </c>
-      <c r="H9" s="6">
-        <v>641</v>
+        <f>1451-1043</f>
+        <v>408</v>
+      </c>
+      <c r="H9" s="5">
+        <v>840</v>
       </c>
       <c r="I9">
-        <f>3.54*J9</f>
-        <v>1309.8</v>
+        <v>370</v>
       </c>
       <c r="J9">
         <v>370</v>
       </c>
       <c r="K9">
-        <v>3.05</v>
+        <v>1.22</v>
       </c>
       <c r="M9">
-        <v>6100</v>
-      </c>
-      <c r="N9">
-        <v>3050</v>
+        <v>1800</v>
       </c>
       <c r="Q9">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+        <v>4.88</v>
+      </c>
+      <c r="R9" s="10">
+        <v>9.7536000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>1451</v>
+        <v>794</v>
       </c>
       <c r="G10">
-        <f>1451-1043</f>
-        <v>408</v>
-      </c>
-      <c r="H10" s="6">
-        <v>840</v>
-      </c>
-      <c r="I10">
-        <v>370</v>
-      </c>
-      <c r="J10">
-        <v>370</v>
-      </c>
-      <c r="K10">
-        <v>1.22</v>
-      </c>
-      <c r="M10">
-        <v>1800</v>
-      </c>
-      <c r="Q10">
-        <v>4.88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>794</v>
-      </c>
-      <c r="G11">
         <f>794-658</f>
         <v>136</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H10" s="5">
         <v>160</v>
       </c>
-      <c r="I11">
-        <f>1.5*J11</f>
+      <c r="I10">
+        <f>1.5*J10</f>
         <v>390</v>
       </c>
-      <c r="J11">
+      <c r="J10">
         <v>260</v>
       </c>
-      <c r="K11">
+      <c r="K10">
         <v>5.18</v>
       </c>
-      <c r="M11">
+      <c r="M10">
         <v>1500</v>
       </c>
-      <c r="Q11">
+      <c r="Q10">
         <v>6.4</v>
       </c>
+      <c r="R10">
+        <v>7.9248000000000003</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{8398FF8C-6382-4DBE-9089-B6764A3E9CB4}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBDF7959-DACF-4FCE-9A50-AD5412DF78C0}">
-  <dimension ref="A2:F3"/>
+  <dimension ref="A2:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" t="s">
         <v>68</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" t="s">
-        <v>70</v>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="8">
+        <f>1.979*B9+1642.6</f>
+        <v>2434.1999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="8">
+        <f>(B10-272.09)/2.6</f>
+        <v>831.58076923076908</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="9">
+        <f>B11-B9</f>
+        <v>431.58076923076908</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="7">
+        <f>0.41*B10-103.31</f>
+        <v>894.71199999999976</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="7">
+        <f>LOG((B13+458.23)/332.32)/0.3</f>
+        <v>2.0324089993379251</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:B8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF59C21-F735-41EF-8378-FF3E9B272E14}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="5"/>
+    <col min="3" max="3" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="5">
+        <v>12284</v>
+      </c>
+      <c r="C2" s="5">
+        <v>24494</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1360</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2910</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1400</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="5">
+        <v>4000</v>
+      </c>
+      <c r="C5" s="5">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="5">
+        <v>5600</v>
+      </c>
+      <c r="C6" s="5">
+        <v>15600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C2FA89-20FA-4B37-9726-5797E5FAD65E}">
   <dimension ref="A2:D10"/>
   <sheetViews>
@@ -1279,7 +2501,7 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2">
         <v>0.01</v>
@@ -1295,7 +2517,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4">
         <f>B3/B9</f>
@@ -1308,7 +2530,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5">
         <f>B3/B10</f>
@@ -1317,7 +2539,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <f>B3*3.721</f>
@@ -1326,7 +2548,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C7">
         <f>SQRT(C6/2/(B2*C4))</f>
@@ -1339,7 +2561,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B9">
         <v>50</v>
@@ -1350,7 +2572,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -1365,15 +2587,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003903DA4920FEBC41BB5F969FFD47B964" ma:contentTypeVersion="12" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="1bae9117eb5db67c45c89f1294bb7f44">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1c2c6ee9-b8be-49d9-90c3-9c81ce8bfa2f" xmlns:ns3="576e201b-6fca-4d2d-97f9-f66e1a2295ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d16cd453913853f302121db62409de4d" ns2:_="" ns3:_="">
     <xsd:import namespace="1c2c6ee9-b8be-49d9-90c3-9c81ce8bfa2f"/>
@@ -1588,6 +2801,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1600,14 +2822,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FE13C52-65DE-436D-A983-C1B2AC891AAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4B45685-B521-4930-B35F-CFAA9724071C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1622,6 +2836,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FE13C52-65DE-436D-A983-C1B2AC891AAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>